<commit_message>
Mapeo de categorias y campos de producto, contruccion del excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive\Documentos\ROBOT MADE\webscraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4A733C-1C58-47BE-8A6D-44C16AC7295C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52BAC1F-5AF2-4F96-A3D2-8F559CBB1E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Categoria 1</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Imagen</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Dimensiones</t>
+  </si>
+  <si>
+    <t>Largo</t>
+  </si>
+  <si>
+    <t>Ancho</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Diametro</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Contenido</t>
   </si>
 </sst>
 </file>
@@ -110,16 +137,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E90B6EA7-24C9-40A2-9EE6-4CD5108B9BD3}" name="Tabla1" displayName="Tabla1" ref="A1:H1048576" totalsRowShown="0">
-  <autoFilter ref="A1:H1048576" xr:uid="{E90B6EA7-24C9-40A2-9EE6-4CD5108B9BD3}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E90B6EA7-24C9-40A2-9EE6-4CD5108B9BD3}" name="Tabla1" displayName="Tabla1" ref="A1:Q1048576" totalsRowShown="0">
+  <autoFilter ref="A1:Q1048576" xr:uid="{E90B6EA7-24C9-40A2-9EE6-4CD5108B9BD3}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{7BD68917-1BB1-458C-AA52-548431FAAA6F}" name="Categoria 1"/>
     <tableColumn id="2" xr3:uid="{4EE04553-CE45-40A6-B1E2-D3C2CE1CDA79}" name="Categoria 2"/>
     <tableColumn id="3" xr3:uid="{30B9A430-9708-42C7-8151-C7469C5CFDC6}" name="Categoria 3"/>
     <tableColumn id="4" xr3:uid="{9A1350B8-F131-4CFF-A36F-43CA3C62F5EC}" name="Categoria 4"/>
     <tableColumn id="5" xr3:uid="{AEA4131D-10C0-4423-91B6-71B720F91365}" name="Categoria 5"/>
-    <tableColumn id="6" xr3:uid="{9ED1438A-5D84-4415-9CBD-EACD522D015F}" name="Nombre"/>
-    <tableColumn id="7" xr3:uid="{ADDE34AA-8FA1-4967-BD95-03BB9066D922}" name="Precio"/>
+    <tableColumn id="11" xr3:uid="{234E432D-FC2B-4D69-A97D-30EDDE7EED22}" name="Marca"/>
+    <tableColumn id="12" xr3:uid="{9FC79C02-7520-47D5-ABE4-C655A105CC98}" name="Nombre"/>
+    <tableColumn id="13" xr3:uid="{F20DCE84-A217-4F39-84DF-24706D8B581C}" name="Precio"/>
+    <tableColumn id="15" xr3:uid="{F7021D82-686D-4E62-89D9-B9A56CC29FE3}" name="Dimensiones"/>
+    <tableColumn id="16" xr3:uid="{6D06C065-4A1B-48B4-9A7D-F0B3DAC3D0AE}" name="Largo"/>
+    <tableColumn id="17" xr3:uid="{9B025D08-AD5F-4272-A7BE-807A2D063A49}" name="Ancho"/>
+    <tableColumn id="14" xr3:uid="{0DFEE663-A4E2-45FB-B27E-A8177AB180B7}" name="Alto"/>
+    <tableColumn id="9" xr3:uid="{EA739629-B65E-4C4C-8662-269DDA7D0611}" name="Diametro"/>
+    <tableColumn id="10" xr3:uid="{4585D58A-1667-4219-8D3C-5D88FC27CAEB}" name="Color"/>
+    <tableColumn id="6" xr3:uid="{9ED1438A-5D84-4415-9CBD-EACD522D015F}" name="Uso"/>
+    <tableColumn id="7" xr3:uid="{ADDE34AA-8FA1-4967-BD95-03BB9066D922}" name="Contenido"/>
     <tableColumn id="8" xr3:uid="{229D1E8F-1885-4439-AF0C-682951D30E39}" name="Imagen"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -389,18 +425,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="11.109375" customWidth="1"/>
+    <col min="1" max="17" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,12 +453,39 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>